<commit_message>
Add Scripts UC_01_BuyTicket (Homework4)
</commit_message>
<xml_diff>
--- a/Documents/Homework3/WebTours Профиль нагрузки (простой) (1).xlsx
+++ b/Documents/Homework3/WebTours Профиль нагрузки (простой) (1).xlsx
@@ -140,13 +140,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0.0"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,69 +163,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,6 +184,21 @@
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -243,26 +206,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -275,6 +236,45 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -283,13 +283,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="204"/>
@@ -313,7 +306,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
@@ -330,7 +323,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,31 +356,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,163 +476,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -645,26 +614,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -693,11 +647,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
       </bottom>
       <diagonal/>
     </border>
@@ -731,108 +709,99 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -847,7 +816,7 @@
     <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -856,7 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1219,7 +1188,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1369,11 +1338,11 @@
         <v>345</v>
       </c>
       <c r="C5" s="5">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="6">
         <f>60/C5</f>
-        <v>1.875</v>
+        <v>1.93548387096774</v>
       </c>
       <c r="E5" s="7">
         <v>60</v>
@@ -1386,12 +1355,12 @@
         <v>3</v>
       </c>
       <c r="H5" s="9">
-        <f>D5*E5*G5</f>
-        <v>337.5</v>
+        <f t="shared" si="1"/>
+        <v>348.387096774194</v>
       </c>
       <c r="I5" s="17">
         <f t="shared" si="2"/>
-        <v>-0.0217391304347826</v>
+        <v>0.00981767180925663</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1419,7 +1388,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="9">
-        <f>D6*E6*G6</f>
+        <f t="shared" si="1"/>
         <v>240</v>
       </c>
       <c r="I6" s="17">

</xml_diff>